<commit_message>
retain data in elevated_risk for hhms
</commit_message>
<xml_diff>
--- a/codebook/var_names_v5.xlsx
+++ b/codebook/var_names_v5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/codebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kw\Documents\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8655CD-4B6F-A549-B64C-700493EE52F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED5DC69-49A3-4C65-B96D-D28ED23C33D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1960" windowWidth="26840" windowHeight="15140" activeTab="1" xr2:uid="{E31ED7E8-A779-9944-B50F-ADC911EBE30D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15480" xr2:uid="{E31ED7E8-A779-9944-B50F-ADC911EBE30D}"/>
   </bookViews>
   <sheets>
     <sheet name="survey_5" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="674">
   <si>
     <t>oldname</t>
   </si>
@@ -1671,9 +1671,6 @@
   </si>
   <si>
     <t>q28a_scale_1</t>
-  </si>
-  <si>
-    <t>repeat_q28_scale</t>
   </si>
   <si>
     <t>variable</t>
@@ -2422,13 +2419,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB98F4A-8635-484F-A746-6470D215D86F}">
   <dimension ref="A1:B297"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
+      <selection activeCell="B272" sqref="B272"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2436,19 +2436,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2496,25 +2496,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -2522,35 +2522,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -2558,19 +2558,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>43</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>45</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>47</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>49</v>
       </c>
@@ -2682,13 +2682,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>52</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>54</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>56</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>58</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>60</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>62</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>64</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>66</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>68</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>72</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>74</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>76</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>78</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>80</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>82</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>84</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>86</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>88</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>90</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>92</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>94</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>96</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>98</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>100</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>102</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>104</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>106</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>108</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>110</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>112</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>114</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>116</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>118</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>120</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>122</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>124</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>126</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>128</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>130</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>132</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>134</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>136</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>138</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>140</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>142</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>144</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>146</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>148</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>150</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>152</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>154</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>156</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>158</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>160</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>162</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>164</v>
       </c>
@@ -3144,7 +3144,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>166</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>168</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>170</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>172</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>174</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>176</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>178</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>180</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>182</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>184</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>185</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>187</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>189</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>191</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>193</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>195</v>
       </c>
@@ -3272,13 +3272,13 @@
         <v>196</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>197</v>
       </c>
       <c r="B110" s="1"/>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>198</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>200</v>
       </c>
@@ -3294,19 +3294,19 @@
         <v>201</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>202</v>
       </c>
       <c r="B113" s="1"/>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>203</v>
       </c>
       <c r="B114" s="1"/>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>204</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>206</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>208</v>
       </c>
@@ -3330,13 +3330,13 @@
         <v>209</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>210</v>
       </c>
       <c r="B118" s="1"/>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>211</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>213</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>215</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>217</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>219</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>221</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>223</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>225</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>227</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>229</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>231</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>233</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>235</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>237</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>239</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>241</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>243</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>245</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>247</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>249</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>251</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>253</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>255</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>257</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>259</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>261</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>263</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>265</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>267</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>269</v>
       </c>
@@ -3576,13 +3576,13 @@
         <v>270</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>271</v>
       </c>
       <c r="B149" s="1"/>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>272</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>274</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>276</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>278</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>280</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>282</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>284</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>286</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>288</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>290</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>292</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>294</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>296</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>298</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>300</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>302</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>304</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>306</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>308</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>310</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>312</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>314</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>316</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>318</v>
       </c>
@@ -3774,19 +3774,19 @@
         <v>319</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>320</v>
       </c>
       <c r="B174" s="1"/>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>321</v>
       </c>
       <c r="B175" s="1"/>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>322</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>324</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>326</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>328</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>330</v>
       </c>
@@ -3826,7 +3826,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>332</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>334</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>336</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>338</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>340</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>342</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>344</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>346</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>348</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>350</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>352</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>354</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>356</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>358</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>360</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>362</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>364</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>366</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>368</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>370</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>372</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>374</v>
       </c>
@@ -4002,7 +4002,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>376</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>377</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>378</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>380</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>382</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>384</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>386</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>388</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>390</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>392</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>393</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>394</v>
       </c>
@@ -4098,43 +4098,43 @@
         <v>394</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>395</v>
       </c>
       <c r="B215" s="1"/>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>396</v>
       </c>
       <c r="B216" s="1"/>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>397</v>
       </c>
       <c r="B217" s="1"/>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>398</v>
       </c>
       <c r="B218" s="1"/>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>399</v>
       </c>
       <c r="B219" s="1"/>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>400</v>
       </c>
       <c r="B220" s="1"/>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>401</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>402</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>404</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>406</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>408</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>410</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>412</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>414</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>416</v>
       </c>
@@ -4206,7 +4206,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>418</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>420</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>422</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>424</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>426</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>428</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>430</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>432</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>434</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>436</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>438</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>440</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>442</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>444</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>446</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>448</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>450</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>452</v>
       </c>
@@ -4350,7 +4350,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>454</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>455</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>457</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>459</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>461</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>462</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>464</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>466</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>468</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>2</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>471</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>473</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>475</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>477</v>
       </c>
@@ -4462,7 +4462,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>479</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>481</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>482</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>484</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>486</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>488</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>490</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>492</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>493</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>495</v>
       </c>
@@ -4542,212 +4542,212 @@
         <v>496</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
+        <v>544</v>
+      </c>
+      <c r="B272" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
         <v>497</v>
       </c>
-      <c r="B272" t="s">
+      <c r="B273" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A273" t="s">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
         <v>499</v>
       </c>
-      <c r="B273" t="s">
+      <c r="B274" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A274" t="s">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
         <v>501</v>
       </c>
-      <c r="B274" t="s">
+      <c r="B275" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A275" t="s">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
         <v>503</v>
       </c>
-      <c r="B275" t="s">
+      <c r="B276" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A276" t="s">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
         <v>505</v>
       </c>
-      <c r="B276" t="s">
+      <c r="B277" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A277" t="s">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
         <v>507</v>
       </c>
-      <c r="B277" t="s">
+      <c r="B278" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A278" t="s">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
         <v>509</v>
       </c>
-      <c r="B278" t="s">
+      <c r="B279" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A279" t="s">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
         <v>511</v>
       </c>
-      <c r="B279" t="s">
+      <c r="B280" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A280" t="s">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
         <v>513</v>
       </c>
-      <c r="B280" t="s">
+      <c r="B281" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A281" t="s">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
         <v>515</v>
       </c>
-      <c r="B281" t="s">
+      <c r="B282" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A282" t="s">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
         <v>517</v>
       </c>
-      <c r="B282" t="s">
+      <c r="B283" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A283" t="s">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
         <v>519</v>
       </c>
-      <c r="B283" t="s">
+      <c r="B284" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A284" t="s">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
         <v>521</v>
       </c>
-      <c r="B284" t="s">
+      <c r="B285" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A285" t="s">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
         <v>523</v>
       </c>
-      <c r="B285" t="s">
+      <c r="B286" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A286" t="s">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
         <v>197</v>
       </c>
-      <c r="B286" t="s">
+      <c r="B287" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A287" t="s">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
         <v>202</v>
       </c>
-      <c r="B287" t="s">
+      <c r="B288" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A288" t="s">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
         <v>203</v>
       </c>
-      <c r="B288" t="s">
+      <c r="B289" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A289" t="s">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
         <v>528</v>
       </c>
-      <c r="B289" s="1" t="s">
+      <c r="B290" s="1" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A290" t="s">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
         <v>530</v>
       </c>
-      <c r="B290" t="s">
+      <c r="B291" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A291" t="s">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
         <v>532</v>
       </c>
-      <c r="B291" t="s">
+      <c r="B292" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A292" t="s">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
         <v>534</v>
       </c>
-      <c r="B292" t="s">
+      <c r="B293" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A293" t="s">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
         <v>536</v>
       </c>
-      <c r="B293" t="s">
+      <c r="B294" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A294" t="s">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
         <v>538</v>
       </c>
-      <c r="B294" t="s">
+      <c r="B295" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A295" t="s">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
         <v>540</v>
       </c>
-      <c r="B295" t="s">
+      <c r="B296" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A296" t="s">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
         <v>542</v>
       </c>
-      <c r="B296" t="s">
+      <c r="B297" t="s">
         <v>543</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A297" t="s">
-        <v>544</v>
-      </c>
-      <c r="B297" t="s">
-        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -4759,18 +4759,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCB9696-9885-3845-AF71-77BCF991F2B8}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -4779,339 +4779,339 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>353</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>353</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>353</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>359</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>359</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>359</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>359</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -5130,606 +5130,606 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" s="1" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102" s="1" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104" s="1" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" s="1" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" s="1" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A109" s="1" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A110" s="1" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" s="1" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115" s="1" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
         <v>673</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
-        <v>674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>